<commit_message>
update : JPA 컬럼 수정
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -89,6 +89,9 @@
     <t>HCP_RENTABLE_PRODUCT_INFO_UID</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>HCP_RENTABLE_PRODUCT_INFO 행 고유키</t>
   </si>
   <si>
@@ -188,9 +191,6 @@
     <t>FRONT_IMAGE_UID</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>HCP_RENTABLE_PRODUCT_IMAGE 행 고유키</t>
   </si>
   <si>
@@ -269,13 +269,13 @@
     <t>제품 대여(손님에게 제공)가 가능한 최초 일시</t>
   </si>
   <si>
-    <t>제품 최종 회수 일시</t>
-  </si>
-  <si>
-    <t>STORAGE_DATETIME</t>
-  </si>
-  <si>
-    <t>제품을 최종 회수하는 일시</t>
+    <t>제품 대여 마지막 일시</t>
+  </si>
+  <si>
+    <t>LAST_RENTABLE_DATETIME</t>
+  </si>
+  <si>
+    <t>제품 대여 마지막 일시 (이때가 대여 마지막 날)</t>
   </si>
   <si>
     <t>예약 가능 설정</t>
@@ -937,13 +937,13 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -951,25 +951,25 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -977,16 +977,16 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -995,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -1003,16 +1003,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -1021,7 +1021,7 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
@@ -1029,16 +1029,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -1047,7 +1047,7 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -1055,16 +1055,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1073,7 +1073,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -1081,16 +1081,16 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -1099,7 +1099,7 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -1107,16 +1107,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -1133,16 +1133,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -1151,7 +1151,7 @@
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -1159,16 +1159,16 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
@@ -1177,7 +1177,7 @@
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16">
@@ -1185,10 +1185,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -1197,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -1415,7 +1415,7 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1467,7 +1467,7 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
@@ -1490,7 +1490,7 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -1516,10 +1516,10 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1551,7 +1551,7 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
@@ -1711,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G39" t="s">
         <v>12</v>
@@ -1728,7 +1728,7 @@
         <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1737,7 +1737,7 @@
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
@@ -1751,16 +1751,16 @@
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -1777,16 +1777,16 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -1795,7 +1795,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43">
@@ -1890,7 +1890,7 @@
         <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -1971,7 +1971,7 @@
         <v>105</v>
       </c>
       <c r="F49" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G49" t="s">
         <v>12</v>
@@ -2404,10 +2404,10 @@
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F69" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G69" t="s">
         <v>12</v>
@@ -2544,7 +2544,7 @@
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -2573,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G77" t="s">
         <v>12</v>
@@ -2719,7 +2719,7 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85">
@@ -2876,7 +2876,7 @@
         <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
docs : database 자료 변경
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="188">
   <si>
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO</t>
   </si>
@@ -185,6 +185,15 @@
     <t>고객에게 보일 상품 소개</t>
   </si>
   <si>
+    <t>예약 결재 정보 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT 행 고유키(결재되지 않았다면 null)</t>
+  </si>
+  <si>
     <t>상품 대표 이미지 테이블 고유번호</t>
   </si>
   <si>
@@ -347,6 +356,9 @@
     <t>RESERVATION_UNIT_PRICE</t>
   </si>
   <si>
+    <t>DECIMAL(15, 2) UNSIGNED</t>
+  </si>
+  <si>
     <t>단위 예약 시간에 대한 가격 (예약 시간 / 단위 예약 시간 * 예약 단가 = 예약 최종가)</t>
   </si>
   <si>
@@ -443,10 +455,10 @@
     <t>HCP_RENTABLE_PRODUCT_STOCK_IMAGE</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_UID</t>
+    <t>HCP_PAYMENT</t>
+  </si>
+  <si>
+    <t>HCP_HCP_PAYMENT_UID</t>
   </si>
   <si>
     <t>결재 타입</t>
@@ -479,13 +491,13 @@
     <t>PAYMENT_FAILED</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_REAL_TIME_TRANSFERS</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_REAL_TIME_TRANSFERS_UID</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_UID2</t>
+    <t>HCP_PAYMENT_REAL_TIME_TRANSFERS</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_REAL_TIME_TRANSFERS_UID</t>
+  </si>
+  <si>
+    <t>결재 정보 고유키</t>
   </si>
   <si>
     <t>입금 은행명</t>
@@ -512,10 +524,10 @@
     <t>DEPOSITOR_NAME</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_VIRTUAL_ACCOUNT_PAY</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_VIRTUAL_ACCOUNT_PAY_UID</t>
+    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY_UID</t>
   </si>
   <si>
     <t>입금 은행 가상 계좌번호</t>
@@ -524,7 +536,43 @@
     <t>VIRTUAL_ACCOUNT_NUMBER</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_TOSS_PAYMENT</t>
+    <t>HCP_PAYMENT_TOSS_PAYMENT</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_TOSS_PAYMENT_UID</t>
+  </si>
+  <si>
+    <t>Toss 거래 아이디</t>
+  </si>
+  <si>
+    <t>TOSS_TRANSACTION_ID</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_REFUND</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_REFUND_UID</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT 행 고유키</t>
+  </si>
+  <si>
+    <t>환불 금액</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>환불 완료 일시</t>
+  </si>
+  <si>
+    <t>REFUND_DATETIME</t>
+  </si>
+  <si>
+    <t>환불 완료한 일시</t>
   </si>
 </sst>
 </file>
@@ -893,7 +941,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:H150"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1292,7 +1340,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
@@ -1304,16 +1352,16 @@
         <v>12</v>
       </c>
       <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
         <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18">
@@ -1321,25 +1369,25 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -1347,16 +1395,16 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
         <v>69</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
         <v>70</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1372,79 +1420,79 @@
       <c r="A20" t="s">
         <v>12</v>
       </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -1453,7 +1501,7 @@
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
@@ -1461,16 +1509,16 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
@@ -1479,38 +1527,38 @@
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>77</v>
@@ -1522,21 +1570,21 @@
         <v>12</v>
       </c>
       <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
         <v>79</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
         <v>80</v>
@@ -1548,21 +1596,21 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
@@ -1574,10 +1622,10 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1603,7 +1651,7 @@
         <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1614,45 +1662,45 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
         <v>14</v>
@@ -1661,86 +1709,86 @@
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
         <v>12</v>
       </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -1749,7 +1797,7 @@
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1757,16 +1805,16 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -1775,33 +1823,33 @@
         <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
         <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40">
@@ -1809,10 +1857,10 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1827,33 +1875,33 @@
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42">
@@ -1861,16 +1909,16 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -1879,7 +1927,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43">
@@ -1887,16 +1935,16 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -1905,7 +1953,7 @@
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44">
@@ -1913,25 +1961,25 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
         <v>65</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
         <v>66</v>
       </c>
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
         <v>67</v>
-      </c>
-      <c r="F44" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45">
@@ -1939,16 +1987,16 @@
         <v>12</v>
       </c>
       <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
         <v>69</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
         <v>70</v>
-      </c>
-      <c r="D45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" t="s">
-        <v>67</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -1965,16 +2013,16 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -1983,7 +2031,7 @@
         <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47">
@@ -2000,7 +2048,7 @@
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F47" t="s">
         <v>14</v>
@@ -2026,16 +2074,16 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
         <v>105</v>
-      </c>
-      <c r="F48" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="49">
@@ -2043,19 +2091,19 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
         <v>107</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
         <v>108</v>
       </c>
-      <c r="D49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" t="s">
-        <v>105</v>
-      </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G49" t="s">
         <v>12</v>
@@ -2078,10 +2126,10 @@
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G50" t="s">
         <v>12</v>
@@ -2095,16 +2143,16 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="F51" t="s">
         <v>14</v>
@@ -2113,86 +2161,86 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
         <v>12</v>
       </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H55" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
         <v>14</v>
@@ -2201,7 +2249,7 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57">
@@ -2209,16 +2257,16 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
@@ -2227,24 +2275,24 @@
         <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F58" t="s">
         <v>14</v>
@@ -2253,24 +2301,24 @@
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
         <v>14</v>
@@ -2305,86 +2353,86 @@
         <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
         <v>12</v>
       </c>
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" t="s">
-        <v>6</v>
-      </c>
-      <c r="G63" t="s">
-        <v>7</v>
-      </c>
-      <c r="H63" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G64" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H64" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -2393,7 +2441,7 @@
         <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66">
@@ -2401,16 +2449,16 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -2419,24 +2467,24 @@
         <v>12</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
@@ -2445,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="H67" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68">
@@ -2453,10 +2501,10 @@
         <v>23</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2471,112 +2519,112 @@
         <v>12</v>
       </c>
       <c r="H68" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C69" t="s">
-        <v>129</v>
+        <v>11</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G69" t="s">
         <v>12</v>
       </c>
       <c r="H69" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
         <v>12</v>
       </c>
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" t="s">
+        <v>133</v>
+      </c>
+      <c r="D70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" t="s">
-        <v>4</v>
-      </c>
-      <c r="E72" t="s">
-        <v>5</v>
-      </c>
-      <c r="F72" t="s">
-        <v>6</v>
-      </c>
-      <c r="G72" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F73" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G73" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H73" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F74" t="s">
         <v>14</v>
@@ -2585,7 +2633,7 @@
         <v>12</v>
       </c>
       <c r="H74" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75">
@@ -2593,16 +2641,16 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F75" t="s">
         <v>14</v>
@@ -2611,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76">
@@ -2619,16 +2667,16 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -2637,112 +2685,112 @@
         <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C77" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F77" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G77" t="s">
         <v>12</v>
       </c>
       <c r="H77" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="B78" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" t="s">
-        <v>6</v>
-      </c>
-      <c r="G80" t="s">
-        <v>7</v>
-      </c>
-      <c r="H80" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G81" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H81" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F82" t="s">
         <v>14</v>
@@ -2751,7 +2799,7 @@
         <v>12</v>
       </c>
       <c r="H82" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83">
@@ -2759,16 +2807,16 @@
         <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
         <v>14</v>
@@ -2777,24 +2825,24 @@
         <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C84" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F84" t="s">
         <v>14</v>
@@ -2803,24 +2851,24 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="F85" t="s">
         <v>14</v>
@@ -2829,86 +2877,86 @@
         <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
         <v>12</v>
       </c>
+      <c r="B86" t="s">
+        <v>141</v>
+      </c>
+      <c r="C86" t="s">
+        <v>142</v>
+      </c>
+      <c r="D86" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>1</v>
-      </c>
-      <c r="B88" t="s">
-        <v>2</v>
-      </c>
-      <c r="C88" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" t="s">
-        <v>4</v>
-      </c>
-      <c r="E88" t="s">
-        <v>5</v>
-      </c>
-      <c r="F88" t="s">
-        <v>6</v>
-      </c>
-      <c r="G88" t="s">
-        <v>7</v>
-      </c>
-      <c r="H88" t="s">
-        <v>8</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F89" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G89" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H89" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D90" t="s">
         <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F90" t="s">
         <v>14</v>
@@ -2917,7 +2965,7 @@
         <v>12</v>
       </c>
       <c r="H90" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91">
@@ -2925,16 +2973,16 @@
         <v>12</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
@@ -2943,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="H91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92">
@@ -2951,16 +2999,16 @@
         <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="C92" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>
@@ -2969,24 +3017,24 @@
         <v>12</v>
       </c>
       <c r="H92" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C93" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F93" t="s">
         <v>14</v>
@@ -2995,86 +3043,86 @@
         <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" t="s">
+        <v>145</v>
+      </c>
+      <c r="D94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" t="s">
+        <v>12</v>
+      </c>
+      <c r="H94" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>1</v>
-      </c>
-      <c r="B96" t="s">
-        <v>2</v>
-      </c>
-      <c r="C96" t="s">
-        <v>3</v>
-      </c>
-      <c r="D96" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96" t="s">
-        <v>5</v>
-      </c>
-      <c r="F96" t="s">
-        <v>6</v>
-      </c>
-      <c r="G96" t="s">
-        <v>7</v>
-      </c>
-      <c r="H96" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E97" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F97" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G97" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H97" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="D98" t="s">
         <v>12</v>
       </c>
       <c r="E98" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F98" t="s">
         <v>14</v>
@@ -3083,7 +3131,7 @@
         <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99">
@@ -3091,16 +3139,16 @@
         <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C99" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
       </c>
       <c r="E99" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F99" t="s">
         <v>14</v>
@@ -3109,24 +3157,24 @@
         <v>12</v>
       </c>
       <c r="H99" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
       </c>
       <c r="E100" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F100" t="s">
         <v>14</v>
@@ -3135,24 +3183,24 @@
         <v>12</v>
       </c>
       <c r="H100" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C101" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="F101" t="s">
         <v>14</v>
@@ -3161,86 +3209,86 @@
         <v>12</v>
       </c>
       <c r="H101" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
         <v>12</v>
       </c>
+      <c r="B102" t="s">
+        <v>141</v>
+      </c>
+      <c r="C102" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" t="s">
-        <v>2</v>
-      </c>
-      <c r="C104" t="s">
-        <v>3</v>
-      </c>
-      <c r="D104" t="s">
-        <v>4</v>
-      </c>
-      <c r="E104" t="s">
-        <v>5</v>
-      </c>
-      <c r="F104" t="s">
-        <v>6</v>
-      </c>
-      <c r="G104" t="s">
-        <v>7</v>
-      </c>
-      <c r="H104" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E105" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F105" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G105" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H105" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C106" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="D106" t="s">
         <v>12</v>
       </c>
       <c r="E106" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F106" t="s">
         <v>14</v>
@@ -3249,7 +3297,7 @@
         <v>12</v>
       </c>
       <c r="H106" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107">
@@ -3257,16 +3305,16 @@
         <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C107" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D107" t="s">
         <v>12</v>
       </c>
       <c r="E107" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3275,24 +3323,24 @@
         <v>12</v>
       </c>
       <c r="H107" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
         <v>12</v>
       </c>
       <c r="E108" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3301,7 +3349,7 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109">
@@ -3309,16 +3357,16 @@
         <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C109" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
       </c>
       <c r="E109" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -3327,7 +3375,7 @@
         <v>12</v>
       </c>
       <c r="H109" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="110">
@@ -3335,16 +3383,16 @@
         <v>12</v>
       </c>
       <c r="B110" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C110" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D110" t="s">
         <v>12</v>
       </c>
       <c r="E110" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="F110" t="s">
         <v>14</v>
@@ -3353,7 +3401,7 @@
         <v>12</v>
       </c>
       <c r="H110" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="111">
@@ -3361,10 +3409,10 @@
         <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C111" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D111" t="s">
         <v>12</v>
@@ -3379,7 +3427,7 @@
         <v>12</v>
       </c>
       <c r="H111" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112">
@@ -3387,10 +3435,10 @@
         <v>12</v>
       </c>
       <c r="B112" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D112" t="s">
         <v>12</v>
@@ -3405,7 +3453,7 @@
         <v>12</v>
       </c>
       <c r="H112" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="113">
@@ -3415,7 +3463,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115">
@@ -3452,7 +3500,7 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
@@ -3527,10 +3575,10 @@
         <v>23</v>
       </c>
       <c r="B119" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="C119" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
@@ -3553,16 +3601,16 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C120" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D120" t="s">
         <v>12</v>
       </c>
       <c r="E120" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F120" t="s">
         <v>14</v>
@@ -3571,7 +3619,7 @@
         <v>12</v>
       </c>
       <c r="H120" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="121">
@@ -3579,16 +3627,16 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C121" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D121" t="s">
         <v>12</v>
       </c>
       <c r="E121" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F121" t="s">
         <v>14</v>
@@ -3597,7 +3645,7 @@
         <v>12</v>
       </c>
       <c r="H121" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122">
@@ -3605,17 +3653,17 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
+        <v>169</v>
+      </c>
+      <c r="C122" t="s">
+        <v>170</v>
+      </c>
+      <c r="D122" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" t="s">
         <v>165</v>
       </c>
-      <c r="C122" t="s">
-        <v>166</v>
-      </c>
-      <c r="D122" t="s">
-        <v>12</v>
-      </c>
-      <c r="E122" t="s">
-        <v>161</v>
-      </c>
       <c r="F122" t="s">
         <v>14</v>
       </c>
@@ -3623,7 +3671,7 @@
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123">
@@ -3633,7 +3681,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="125">
@@ -3670,7 +3718,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D126" t="s">
         <v>12</v>
@@ -3745,10 +3793,10 @@
         <v>23</v>
       </c>
       <c r="B129" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="C129" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
@@ -3771,16 +3819,16 @@
         <v>12</v>
       </c>
       <c r="B130" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C130" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
       </c>
       <c r="E130" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F130" t="s">
         <v>14</v>
@@ -3789,7 +3837,7 @@
         <v>12</v>
       </c>
       <c r="H130" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131">
@@ -3797,16 +3845,16 @@
         <v>12</v>
       </c>
       <c r="B131" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C131" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
       </c>
       <c r="E131" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F131" t="s">
         <v>14</v>
@@ -3815,7 +3863,7 @@
         <v>12</v>
       </c>
       <c r="H131" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="132">
@@ -3823,17 +3871,17 @@
         <v>12</v>
       </c>
       <c r="B132" t="s">
+        <v>169</v>
+      </c>
+      <c r="C132" t="s">
+        <v>170</v>
+      </c>
+      <c r="D132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132" t="s">
         <v>165</v>
       </c>
-      <c r="C132" t="s">
-        <v>166</v>
-      </c>
-      <c r="D132" t="s">
-        <v>12</v>
-      </c>
-      <c r="E132" t="s">
-        <v>161</v>
-      </c>
       <c r="F132" t="s">
         <v>14</v>
       </c>
@@ -3841,7 +3889,7 @@
         <v>12</v>
       </c>
       <c r="H132" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133">
@@ -3851,7 +3899,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="135">
@@ -3888,7 +3936,7 @@
         <v>10</v>
       </c>
       <c r="C136" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D136" t="s">
         <v>12</v>
@@ -3963,10 +4011,10 @@
         <v>23</v>
       </c>
       <c r="B139" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="C139" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
@@ -3989,16 +4037,16 @@
         <v>12</v>
       </c>
       <c r="B140" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="C140" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
       </c>
       <c r="E140" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="F140" t="s">
         <v>14</v>
@@ -4007,63 +4055,203 @@
         <v>12</v>
       </c>
       <c r="H140" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" t="s">
-        <v>169</v>
-      </c>
-      <c r="C141" t="s">
-        <v>170</v>
-      </c>
-      <c r="D141" t="s">
-        <v>12</v>
-      </c>
-      <c r="E141" t="s">
-        <v>164</v>
-      </c>
-      <c r="F141" t="s">
-        <v>14</v>
-      </c>
-      <c r="G141" t="s">
-        <v>12</v>
-      </c>
-      <c r="H141" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>12</v>
-      </c>
-      <c r="B142" t="s">
-        <v>165</v>
-      </c>
-      <c r="C142" t="s">
-        <v>166</v>
-      </c>
-      <c r="D142" t="s">
-        <v>12</v>
-      </c>
-      <c r="E142" t="s">
-        <v>161</v>
-      </c>
-      <c r="F142" t="s">
-        <v>14</v>
-      </c>
-      <c r="G142" t="s">
-        <v>12</v>
-      </c>
-      <c r="H142" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" t="s">
+        <v>5</v>
+      </c>
+      <c r="F143" t="s">
+        <v>6</v>
+      </c>
+      <c r="G143" t="s">
+        <v>7</v>
+      </c>
+      <c r="H143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>181</v>
+      </c>
+      <c r="D144" t="s">
+        <v>12</v>
+      </c>
+      <c r="E144" t="s">
+        <v>13</v>
+      </c>
+      <c r="F144" t="s">
+        <v>14</v>
+      </c>
+      <c r="G144" t="s">
+        <v>12</v>
+      </c>
+      <c r="H144" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>12</v>
+      </c>
+      <c r="B145" t="s">
+        <v>16</v>
+      </c>
+      <c r="C145" t="s">
+        <v>17</v>
+      </c>
+      <c r="D145" t="s">
+        <v>12</v>
+      </c>
+      <c r="E145" t="s">
+        <v>18</v>
+      </c>
+      <c r="F145" t="s">
+        <v>14</v>
+      </c>
+      <c r="G145" t="s">
+        <v>12</v>
+      </c>
+      <c r="H145" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>20</v>
+      </c>
+      <c r="C146" t="s">
+        <v>21</v>
+      </c>
+      <c r="D146" t="s">
+        <v>12</v>
+      </c>
+      <c r="E146" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" t="s">
+        <v>14</v>
+      </c>
+      <c r="G146" t="s">
+        <v>12</v>
+      </c>
+      <c r="H146" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" t="s">
+        <v>162</v>
+      </c>
+      <c r="C147" t="s">
+        <v>149</v>
+      </c>
+      <c r="D147" t="s">
+        <v>12</v>
+      </c>
+      <c r="E147" t="s">
+        <v>13</v>
+      </c>
+      <c r="F147" t="s">
+        <v>14</v>
+      </c>
+      <c r="G147" t="s">
+        <v>12</v>
+      </c>
+      <c r="H147" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" t="s">
+        <v>183</v>
+      </c>
+      <c r="C148" t="s">
+        <v>184</v>
+      </c>
+      <c r="D148" t="s">
+        <v>12</v>
+      </c>
+      <c r="E148" t="s">
+        <v>115</v>
+      </c>
+      <c r="F148" t="s">
+        <v>14</v>
+      </c>
+      <c r="G148" t="s">
+        <v>12</v>
+      </c>
+      <c r="H148" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>12</v>
+      </c>
+      <c r="B149" t="s">
+        <v>185</v>
+      </c>
+      <c r="C149" t="s">
+        <v>186</v>
+      </c>
+      <c r="D149" t="s">
+        <v>12</v>
+      </c>
+      <c r="E149" t="s">
+        <v>22</v>
+      </c>
+      <c r="F149" t="s">
+        <v>26</v>
+      </c>
+      <c r="G149" t="s">
+        <v>12</v>
+      </c>
+      <c r="H149" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update : 정보 수정
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -374,10 +374,10 @@
     <t>업데이트 버전 시퀀스 (0에서 시작해서 정보 업데이트가 될 때마다 1 씩 올라갑니다. 예약 프로세스 진행중 버전 정보가 맞지 않으면 진행이 불가능하게 할 것.)</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_INFO</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_INFO_UID</t>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY_UID</t>
   </si>
   <si>
     <t>대여 가능 상품 예약 정보 고유키</t>

</xml_diff>

<commit_message>
update : 설계 수정
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="197">
   <si>
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO</t>
   </si>
@@ -143,16 +143,7 @@
     <t>PAYMENT_DEADLINE_DATETIME</t>
   </si>
   <si>
-    <t>예약 결재 기한 (예약 요청일로부터 생성, 이 시점이 지났고, payment_complete_datetime 가 충족되지 않았다면 취소로 간주)</t>
-  </si>
-  <si>
-    <t>예약 취소 신청 가능 기한</t>
-  </si>
-  <si>
-    <t>CANCELABLE_DEADLINE_DATETIME</t>
-  </si>
-  <si>
-    <t>예약 요청일로부터 생성, 예약 취소 신청 가능 기한</t>
+    <t>예약 결재 기한 (결재 기한 초과 처리.)</t>
   </si>
   <si>
     <t>관리자 승인 기한</t>
@@ -977,7 +968,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H161"/>
+  <dimension ref="A1:H160"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1284,7 +1275,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -1310,7 +1301,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -1319,27 +1310,27 @@
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -1350,7 +1341,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>58</v>
@@ -1362,16 +1353,16 @@
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
@@ -1379,16 +1370,16 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -1397,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18">
@@ -1405,16 +1396,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -1430,79 +1421,79 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
@@ -1511,7 +1502,7 @@
         <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
@@ -1519,16 +1510,16 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -1537,38 +1528,38 @@
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>74</v>
@@ -1580,21 +1571,21 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>77</v>
@@ -1606,21 +1597,21 @@
         <v>12</v>
       </c>
       <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
         <v>79</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
         <v>80</v>
@@ -1632,10 +1623,10 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
@@ -1661,7 +1652,7 @@
         <v>37</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1672,45 +1663,45 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
@@ -1719,86 +1710,86 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -1807,7 +1798,7 @@
         <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37">
@@ -1815,16 +1806,16 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -1833,33 +1824,33 @@
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39">
@@ -1867,10 +1858,10 @@
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -1885,33 +1876,33 @@
         <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41">
@@ -1928,7 +1919,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -1937,7 +1928,7 @@
         <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42">
@@ -1945,16 +1936,16 @@
         <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -1963,7 +1954,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43">
@@ -1971,16 +1962,16 @@
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -1989,7 +1980,7 @@
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44">
@@ -1997,16 +1988,16 @@
         <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F44" t="s">
         <v>14</v>
@@ -2023,16 +2014,16 @@
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -2041,7 +2032,7 @@
         <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46">
@@ -2058,7 +2049,7 @@
         <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -2084,7 +2075,7 @@
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="F47" t="s">
         <v>14</v>
@@ -2093,7 +2084,7 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48">
@@ -2101,19 +2092,19 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G48" t="s">
         <v>12</v>
@@ -2136,16 +2127,16 @@
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G49" t="s">
         <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50">
@@ -2153,16 +2144,16 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F50" t="s">
         <v>14</v>
@@ -2171,7 +2162,7 @@
         <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51">
@@ -2179,16 +2170,16 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="F51" t="s">
         <v>14</v>
@@ -2197,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52">
@@ -2205,16 +2196,16 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="F52" t="s">
         <v>14</v>
@@ -2223,86 +2214,86 @@
         <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
         <v>12</v>
       </c>
-      <c r="B53" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
-        <v>105</v>
-      </c>
-      <c r="F53" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
@@ -2311,7 +2302,7 @@
         <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58">
@@ -2319,16 +2310,16 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F58" t="s">
         <v>14</v>
@@ -2337,24 +2328,24 @@
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
         <v>14</v>
@@ -2363,24 +2354,24 @@
         <v>12</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
         <v>123</v>
       </c>
-      <c r="C60" t="s">
-        <v>11</v>
-      </c>
       <c r="D60" t="s">
         <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="F60" t="s">
         <v>14</v>
@@ -2389,7 +2380,7 @@
         <v>12</v>
       </c>
       <c r="H60" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61">
@@ -2397,104 +2388,104 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" t="s">
         <v>126</v>
-      </c>
-      <c r="D61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" t="s">
-        <v>127</v>
-      </c>
-      <c r="F61" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" t="s">
-        <v>12</v>
-      </c>
-      <c r="H61" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
         <v>12</v>
       </c>
-      <c r="B62" t="s">
-        <v>129</v>
-      </c>
-      <c r="C62" t="s">
-        <v>130</v>
-      </c>
-      <c r="D62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" t="s">
-        <v>131</v>
-      </c>
-      <c r="F62" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" t="s">
-        <v>12</v>
-      </c>
-      <c r="H62" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G65" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -2503,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="H66" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67">
@@ -2511,16 +2502,16 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F67" t="s">
         <v>14</v>
@@ -2529,24 +2520,24 @@
         <v>12</v>
       </c>
       <c r="H67" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
@@ -2555,7 +2546,7 @@
         <v>12</v>
       </c>
       <c r="H68" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69">
@@ -2563,10 +2554,10 @@
         <v>23</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -2581,112 +2572,112 @@
         <v>12</v>
       </c>
       <c r="H69" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F70" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G70" t="s">
         <v>12</v>
       </c>
       <c r="H70" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
         <v>12</v>
       </c>
-      <c r="B71" t="s">
-        <v>136</v>
-      </c>
-      <c r="C71" t="s">
-        <v>137</v>
-      </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" t="s">
-        <v>37</v>
-      </c>
-      <c r="F71" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" t="s">
-        <v>12</v>
-      </c>
-      <c r="H71" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D74" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G74" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H74" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F75" t="s">
         <v>14</v>
@@ -2695,7 +2686,7 @@
         <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76">
@@ -2703,16 +2694,16 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -2721,7 +2712,7 @@
         <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77">
@@ -2729,16 +2720,16 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="C77" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F77" t="s">
         <v>14</v>
@@ -2747,112 +2738,112 @@
         <v>12</v>
       </c>
       <c r="H77" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B78" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" t="s">
         <v>140</v>
       </c>
-      <c r="C78" t="s">
-        <v>141</v>
-      </c>
       <c r="D78" t="s">
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F78" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G78" t="s">
         <v>12</v>
       </c>
       <c r="H78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" t="s">
-        <v>142</v>
-      </c>
-      <c r="C79" t="s">
-        <v>143</v>
-      </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" t="s">
-        <v>26</v>
-      </c>
-      <c r="G79" t="s">
-        <v>12</v>
-      </c>
-      <c r="H79" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D82" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F82" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G82" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H82" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F83" t="s">
         <v>14</v>
@@ -2861,7 +2852,7 @@
         <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84">
@@ -2869,16 +2860,16 @@
         <v>12</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C84" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F84" t="s">
         <v>14</v>
@@ -2887,24 +2878,24 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F85" t="s">
         <v>14</v>
@@ -2913,24 +2904,24 @@
         <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>142</v>
       </c>
       <c r="C86" t="s">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
@@ -2939,86 +2930,86 @@
         <v>12</v>
       </c>
       <c r="H86" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
         <v>12</v>
       </c>
-      <c r="B87" t="s">
-        <v>145</v>
-      </c>
-      <c r="C87" t="s">
-        <v>146</v>
-      </c>
-      <c r="D87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E87" t="s">
-        <v>147</v>
-      </c>
-      <c r="F87" t="s">
-        <v>14</v>
-      </c>
-      <c r="G87" t="s">
-        <v>12</v>
-      </c>
-      <c r="H87" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>148</v>
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" t="s">
+        <v>6</v>
+      </c>
+      <c r="G89" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D90" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F90" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G90" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H90" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
@@ -3027,7 +3018,7 @@
         <v>12</v>
       </c>
       <c r="H91" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92">
@@ -3035,16 +3026,16 @@
         <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C92" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>
@@ -3053,7 +3044,7 @@
         <v>12</v>
       </c>
       <c r="H92" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93">
@@ -3061,16 +3052,16 @@
         <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F93" t="s">
         <v>14</v>
@@ -3079,24 +3070,24 @@
         <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D94" t="s">
         <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F94" t="s">
         <v>14</v>
@@ -3105,86 +3096,86 @@
         <v>12</v>
       </c>
       <c r="H94" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>23</v>
-      </c>
-      <c r="B95" t="s">
-        <v>142</v>
-      </c>
-      <c r="C95" t="s">
-        <v>149</v>
-      </c>
-      <c r="D95" t="s">
-        <v>12</v>
-      </c>
-      <c r="E95" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" t="s">
-        <v>12</v>
-      </c>
-      <c r="H95" t="s">
-        <v>150</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>151</v>
+        <v>1</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+      <c r="G97" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D98" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F98" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G98" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C99" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
       </c>
       <c r="E99" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F99" t="s">
         <v>14</v>
@@ -3193,7 +3184,7 @@
         <v>12</v>
       </c>
       <c r="H99" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100">
@@ -3201,16 +3192,16 @@
         <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
       </c>
       <c r="E100" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F100" t="s">
         <v>14</v>
@@ -3219,24 +3210,24 @@
         <v>12</v>
       </c>
       <c r="H100" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F101" t="s">
         <v>14</v>
@@ -3245,24 +3236,24 @@
         <v>12</v>
       </c>
       <c r="H101" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C102" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
       </c>
       <c r="E102" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="F102" t="s">
         <v>14</v>
@@ -3271,86 +3262,86 @@
         <v>12</v>
       </c>
       <c r="H102" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
         <v>12</v>
       </c>
-      <c r="B103" t="s">
-        <v>145</v>
-      </c>
-      <c r="C103" t="s">
-        <v>146</v>
-      </c>
-      <c r="D103" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" t="s">
-        <v>147</v>
-      </c>
-      <c r="F103" t="s">
-        <v>14</v>
-      </c>
-      <c r="G103" t="s">
-        <v>12</v>
-      </c>
-      <c r="H103" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>152</v>
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="D106" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E106" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F106" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G106" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H106" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C107" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
       <c r="D107" t="s">
         <v>12</v>
       </c>
       <c r="E107" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F107" t="s">
         <v>14</v>
@@ -3359,7 +3350,7 @@
         <v>12</v>
       </c>
       <c r="H107" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108">
@@ -3367,16 +3358,16 @@
         <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C108" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
         <v>12</v>
       </c>
       <c r="E108" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
@@ -3385,7 +3376,7 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109">
@@ -3393,16 +3384,16 @@
         <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C109" t="s">
-        <v>21</v>
+        <v>152</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
       </c>
       <c r="E109" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -3411,7 +3402,7 @@
         <v>12</v>
       </c>
       <c r="H109" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110">
@@ -3428,7 +3419,7 @@
         <v>12</v>
       </c>
       <c r="E110" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="F110" t="s">
         <v>14</v>
@@ -3437,7 +3428,7 @@
         <v>12</v>
       </c>
       <c r="H110" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111">
@@ -3445,25 +3436,25 @@
         <v>12</v>
       </c>
       <c r="B111" t="s">
+        <v>156</v>
+      </c>
+      <c r="C111" t="s">
         <v>157</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" t="s">
+        <v>113</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>12</v>
+      </c>
+      <c r="H111" t="s">
         <v>158</v>
-      </c>
-      <c r="D111" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" t="s">
-        <v>112</v>
-      </c>
-      <c r="F111" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" t="s">
-        <v>12</v>
-      </c>
-      <c r="H111" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="112">
@@ -3480,10 +3471,10 @@
         <v>12</v>
       </c>
       <c r="E112" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="F112" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G112" t="s">
         <v>12</v>
@@ -3506,95 +3497,95 @@
         <v>12</v>
       </c>
       <c r="E113" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F113" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G113" t="s">
         <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
         <v>12</v>
       </c>
-      <c r="B114" t="s">
-        <v>165</v>
-      </c>
-      <c r="C114" t="s">
-        <v>166</v>
-      </c>
-      <c r="D114" t="s">
-        <v>12</v>
-      </c>
-      <c r="E114" t="s">
-        <v>18</v>
-      </c>
-      <c r="F114" t="s">
-        <v>14</v>
-      </c>
-      <c r="G114" t="s">
-        <v>12</v>
-      </c>
-      <c r="H114" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>1</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>3</v>
+      </c>
+      <c r="D116" t="s">
+        <v>4</v>
+      </c>
+      <c r="E116" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" t="s">
+        <v>6</v>
+      </c>
+      <c r="G116" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>3</v>
+        <v>165</v>
       </c>
       <c r="D117" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F117" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H117" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C118" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F118" t="s">
         <v>14</v>
@@ -3603,7 +3594,7 @@
         <v>12</v>
       </c>
       <c r="H118" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="119">
@@ -3611,16 +3602,16 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C119" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
       </c>
       <c r="E119" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F119" t="s">
         <v>14</v>
@@ -3629,24 +3620,24 @@
         <v>12</v>
       </c>
       <c r="H119" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="D120" t="s">
         <v>12</v>
       </c>
       <c r="E120" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F120" t="s">
         <v>14</v>
@@ -3655,25 +3646,25 @@
         <v>12</v>
       </c>
       <c r="H120" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
+        <v>167</v>
+      </c>
+      <c r="C121" t="s">
+        <v>168</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
         <v>169</v>
       </c>
-      <c r="C121" t="s">
-        <v>153</v>
-      </c>
-      <c r="D121" t="s">
-        <v>12</v>
-      </c>
-      <c r="E121" t="s">
-        <v>13</v>
-      </c>
       <c r="F121" t="s">
         <v>14</v>
       </c>
@@ -3681,7 +3672,7 @@
         <v>12</v>
       </c>
       <c r="H121" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
     </row>
     <row r="122">
@@ -3724,7 +3715,7 @@
         <v>12</v>
       </c>
       <c r="E123" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F123" t="s">
         <v>14</v>
@@ -3740,79 +3731,79 @@
       <c r="A124" t="s">
         <v>12</v>
       </c>
-      <c r="B124" t="s">
-        <v>176</v>
-      </c>
-      <c r="C124" t="s">
-        <v>177</v>
-      </c>
-      <c r="D124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E124" t="s">
-        <v>172</v>
-      </c>
-      <c r="F124" t="s">
-        <v>14</v>
-      </c>
-      <c r="G124" t="s">
-        <v>12</v>
-      </c>
-      <c r="H124" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>178</v>
+        <v>1</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>4</v>
+      </c>
+      <c r="E126" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" t="s">
+        <v>6</v>
+      </c>
+      <c r="G126" t="s">
+        <v>7</v>
+      </c>
+      <c r="H126" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B127" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C127" t="s">
-        <v>3</v>
+        <v>176</v>
       </c>
       <c r="D127" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E127" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F127" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G127" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H127" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C128" t="s">
-        <v>179</v>
+        <v>17</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
       </c>
       <c r="E128" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F128" t="s">
         <v>14</v>
@@ -3821,7 +3812,7 @@
         <v>12</v>
       </c>
       <c r="H128" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="129">
@@ -3829,16 +3820,16 @@
         <v>12</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
       </c>
       <c r="E129" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F129" t="s">
         <v>14</v>
@@ -3847,24 +3838,24 @@
         <v>12</v>
       </c>
       <c r="H129" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="C130" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
       </c>
       <c r="E130" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F130" t="s">
         <v>14</v>
@@ -3873,25 +3864,25 @@
         <v>12</v>
       </c>
       <c r="H130" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B131" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" t="s">
+        <v>168</v>
+      </c>
+      <c r="D131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131" t="s">
         <v>169</v>
       </c>
-      <c r="C131" t="s">
-        <v>153</v>
-      </c>
-      <c r="D131" t="s">
-        <v>12</v>
-      </c>
-      <c r="E131" t="s">
-        <v>13</v>
-      </c>
       <c r="F131" t="s">
         <v>14</v>
       </c>
@@ -3899,7 +3890,7 @@
         <v>12</v>
       </c>
       <c r="H131" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132">
@@ -3907,10 +3898,10 @@
         <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C132" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
@@ -3933,16 +3924,16 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C133" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D133" t="s">
         <v>12</v>
       </c>
       <c r="E133" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F133" t="s">
         <v>14</v>
@@ -3958,79 +3949,79 @@
       <c r="A134" t="s">
         <v>12</v>
       </c>
-      <c r="B134" t="s">
-        <v>176</v>
-      </c>
-      <c r="C134" t="s">
-        <v>177</v>
-      </c>
-      <c r="D134" t="s">
-        <v>12</v>
-      </c>
-      <c r="E134" t="s">
-        <v>172</v>
-      </c>
-      <c r="F134" t="s">
-        <v>14</v>
-      </c>
-      <c r="G134" t="s">
-        <v>12</v>
-      </c>
-      <c r="H134" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>182</v>
+        <v>1</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" t="s">
+        <v>3</v>
+      </c>
+      <c r="D136" t="s">
+        <v>4</v>
+      </c>
+      <c r="E136" t="s">
+        <v>5</v>
+      </c>
+      <c r="F136" t="s">
+        <v>6</v>
+      </c>
+      <c r="G136" t="s">
+        <v>7</v>
+      </c>
+      <c r="H136" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C137" t="s">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="D137" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E137" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F137" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G137" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H137" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B138" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C138" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="D138" t="s">
         <v>12</v>
       </c>
       <c r="E138" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F138" t="s">
         <v>14</v>
@@ -4039,7 +4030,7 @@
         <v>12</v>
       </c>
       <c r="H138" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="139">
@@ -4047,16 +4038,16 @@
         <v>12</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C139" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
       </c>
       <c r="E139" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F139" t="s">
         <v>14</v>
@@ -4065,24 +4056,24 @@
         <v>12</v>
       </c>
       <c r="H139" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B140" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="C140" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
       </c>
       <c r="E140" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F140" t="s">
         <v>14</v>
@@ -4091,24 +4082,24 @@
         <v>12</v>
       </c>
       <c r="H140" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B141" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C141" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="D141" t="s">
         <v>12</v>
       </c>
       <c r="E141" t="s">
-        <v>13</v>
+        <v>183</v>
       </c>
       <c r="F141" t="s">
         <v>14</v>
@@ -4117,86 +4108,86 @@
         <v>12</v>
       </c>
       <c r="H141" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" t="s">
-        <v>184</v>
-      </c>
-      <c r="C142" t="s">
-        <v>185</v>
-      </c>
-      <c r="D142" t="s">
-        <v>12</v>
-      </c>
-      <c r="E142" t="s">
-        <v>186</v>
-      </c>
-      <c r="F142" t="s">
-        <v>14</v>
-      </c>
-      <c r="G142" t="s">
-        <v>12</v>
-      </c>
-      <c r="H142" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>187</v>
+        <v>1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2</v>
+      </c>
+      <c r="C144" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" t="s">
+        <v>4</v>
+      </c>
+      <c r="E144" t="s">
+        <v>5</v>
+      </c>
+      <c r="F144" t="s">
+        <v>6</v>
+      </c>
+      <c r="G144" t="s">
+        <v>7</v>
+      </c>
+      <c r="H144" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C145" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="D145" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E145" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F145" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G145" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H145" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C146" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="D146" t="s">
         <v>12</v>
       </c>
       <c r="E146" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F146" t="s">
         <v>14</v>
@@ -4205,7 +4196,7 @@
         <v>12</v>
       </c>
       <c r="H146" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="147">
@@ -4213,16 +4204,16 @@
         <v>12</v>
       </c>
       <c r="B147" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C147" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D147" t="s">
         <v>12</v>
       </c>
       <c r="E147" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F147" t="s">
         <v>14</v>
@@ -4231,24 +4222,24 @@
         <v>12</v>
       </c>
       <c r="H147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B148" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="C148" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="D148" t="s">
         <v>12</v>
       </c>
       <c r="E148" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F148" t="s">
         <v>14</v>
@@ -4257,24 +4248,24 @@
         <v>12</v>
       </c>
       <c r="H148" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B149" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="C149" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="D149" t="s">
         <v>12</v>
       </c>
       <c r="E149" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="F149" t="s">
         <v>14</v>
@@ -4283,7 +4274,7 @@
         <v>12</v>
       </c>
       <c r="H149" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="150">
@@ -4291,25 +4282,25 @@
         <v>12</v>
       </c>
       <c r="B150" t="s">
+        <v>189</v>
+      </c>
+      <c r="C150" t="s">
         <v>190</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
+        <v>12</v>
+      </c>
+      <c r="E150" t="s">
+        <v>113</v>
+      </c>
+      <c r="F150" t="s">
+        <v>26</v>
+      </c>
+      <c r="G150" t="s">
+        <v>12</v>
+      </c>
+      <c r="H150" t="s">
         <v>191</v>
-      </c>
-      <c r="D150" t="s">
-        <v>12</v>
-      </c>
-      <c r="E150" t="s">
-        <v>112</v>
-      </c>
-      <c r="F150" t="s">
-        <v>14</v>
-      </c>
-      <c r="G150" t="s">
-        <v>12</v>
-      </c>
-      <c r="H150" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="151">
@@ -4326,7 +4317,7 @@
         <v>12</v>
       </c>
       <c r="E151" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="F151" t="s">
         <v>26</v>
@@ -4342,79 +4333,79 @@
       <c r="A152" t="s">
         <v>12</v>
       </c>
-      <c r="B152" t="s">
-        <v>195</v>
-      </c>
-      <c r="C152" t="s">
-        <v>196</v>
-      </c>
-      <c r="D152" t="s">
-        <v>12</v>
-      </c>
-      <c r="E152" t="s">
-        <v>22</v>
-      </c>
-      <c r="F152" t="s">
-        <v>26</v>
-      </c>
-      <c r="G152" t="s">
-        <v>12</v>
-      </c>
-      <c r="H152" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>12</v>
+        <v>195</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>198</v>
+        <v>1</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>3</v>
+      </c>
+      <c r="D154" t="s">
+        <v>4</v>
+      </c>
+      <c r="E154" t="s">
+        <v>5</v>
+      </c>
+      <c r="F154" t="s">
+        <v>6</v>
+      </c>
+      <c r="G154" t="s">
+        <v>7</v>
+      </c>
+      <c r="H154" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B155" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C155" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="D155" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E155" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F155" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G155" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H155" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B156" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C156" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="D156" t="s">
         <v>12</v>
       </c>
       <c r="E156" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F156" t="s">
         <v>14</v>
@@ -4423,7 +4414,7 @@
         <v>12</v>
       </c>
       <c r="H156" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="157">
@@ -4431,16 +4422,16 @@
         <v>12</v>
       </c>
       <c r="B157" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C157" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
       </c>
       <c r="E157" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F157" t="s">
         <v>14</v>
@@ -4449,24 +4440,24 @@
         <v>12</v>
       </c>
       <c r="H157" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B158" t="s">
-        <v>20</v>
+        <v>196</v>
       </c>
       <c r="C158" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D158" t="s">
         <v>12</v>
       </c>
       <c r="E158" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F158" t="s">
         <v>14</v>
@@ -4475,7 +4466,7 @@
         <v>12</v>
       </c>
       <c r="H158" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
     </row>
     <row r="159">
@@ -4483,10 +4474,10 @@
         <v>23</v>
       </c>
       <c r="B159" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="C159" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="D159" t="s">
         <v>12</v>
@@ -4501,37 +4492,11 @@
         <v>12</v>
       </c>
       <c r="H159" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>23</v>
-      </c>
-      <c r="B160" t="s">
-        <v>169</v>
-      </c>
-      <c r="C160" t="s">
-        <v>153</v>
-      </c>
-      <c r="D160" t="s">
-        <v>12</v>
-      </c>
-      <c r="E160" t="s">
-        <v>13</v>
-      </c>
-      <c r="F160" t="s">
-        <v>14</v>
-      </c>
-      <c r="G160" t="s">
-        <v>12</v>
-      </c>
-      <c r="H160" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs : 결재 -> 결제
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="199">
   <si>
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO</t>
   </si>
@@ -464,111 +464,117 @@
     <t>HCP_HCP_PAYMENT_UID</t>
   </si>
   <si>
-    <t>결재 타입</t>
+    <t>결제 타입</t>
   </si>
   <si>
     <t>PAYMENT_TYPE</t>
   </si>
   <si>
-    <t>결재 타입(1 : 무통장 입금, 2 : 실시간 계좌이체, 3 : 토스 페이)</t>
-  </si>
-  <si>
-    <t>결재 금액</t>
+    <t>결제 타입(1 : 무통장 입금, 2 : 실시간 계좌이체, 3 : 토스 페이)</t>
+  </si>
+  <si>
+    <t>결제 금액</t>
   </si>
   <si>
     <t>PAYMENT_AMOUNT</t>
   </si>
   <si>
-    <t>결재 금액 통화 코드</t>
+    <t>결제 금액 통화 코드</t>
   </si>
   <si>
     <t>PAYMENT_CURRENCY_CODE</t>
   </si>
   <si>
-    <t>결재 금액 통화 코드(IOS 4217, ex : KRW, USD, EUR...)</t>
-  </si>
-  <si>
-    <t>결재 완료 일시</t>
+    <t>결제 금액 통화 코드(IOS 4217, ex : KRW, USD, EUR...)</t>
+  </si>
+  <si>
+    <t>결제 완료 일시</t>
   </si>
   <si>
     <t>PAYMENT_COMPLETE_DATETIME</t>
   </si>
   <si>
-    <t>결재가 완료 및 확인 된 일시(Null 이라면 아직 완료 처리가 아님)</t>
-  </si>
-  <si>
-    <t>결재 실패 여부</t>
+    <t>결제가 완료 및 확인 된 일시(Null 이라면 아직 완료 처리가 아님)</t>
+  </si>
+  <si>
+    <t>결제 실패 여부</t>
   </si>
   <si>
     <t>PAYMENT_FAILED</t>
   </si>
   <si>
+    <t>결제4 실패 여부</t>
+  </si>
+  <si>
     <t>HCP_PAYMENT_REAL_TIME_TRANSFERS</t>
   </si>
   <si>
     <t>HCP_PAYMENT_REAL_TIME_TRANSFERS_UID</t>
   </si>
   <si>
+    <t>결제 정보 고유키</t>
+  </si>
+  <si>
+    <t>입금 은행명</t>
+  </si>
+  <si>
+    <t>BANK_NAME</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>입금 은행 계좌번호</t>
+  </si>
+  <si>
+    <t>ACCOUNT_NUMBER</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>입금자명</t>
+  </si>
+  <si>
+    <t>DEPOSITOR_NAME</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY_UID</t>
+  </si>
+  <si>
+    <t>입금 은행 가상 계좌번호</t>
+  </si>
+  <si>
+    <t>VIRTUAL_ACCOUNT_NUMBER</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_TOSS_PAYMENT</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_TOSS_PAYMENT_UID</t>
+  </si>
+  <si>
+    <t>Toss 거래 아이디</t>
+  </si>
+  <si>
+    <t>TOSS_TRANSACTION_ID</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_REFUND</t>
+  </si>
+  <si>
+    <t>HCP_PAYMENT_REFUND_UID</t>
+  </si>
+  <si>
     <t>결재 정보 고유키</t>
   </si>
   <si>
-    <t>입금 은행명</t>
-  </si>
-  <si>
-    <t>BANK_NAME</t>
-  </si>
-  <si>
-    <t>VARCHAR(100)</t>
-  </si>
-  <si>
-    <t>입금 은행 계좌번호</t>
-  </si>
-  <si>
-    <t>ACCOUNT_NUMBER</t>
-  </si>
-  <si>
-    <t>VARCHAR(50)</t>
-  </si>
-  <si>
-    <t>입금자명</t>
-  </si>
-  <si>
-    <t>DEPOSITOR_NAME</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_VIRTUAL_ACCOUNT_PAY_UID</t>
-  </si>
-  <si>
-    <t>입금 은행 가상 계좌번호</t>
-  </si>
-  <si>
-    <t>VIRTUAL_ACCOUNT_NUMBER</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_TOSS_PAYMENT</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_TOSS_PAYMENT_UID</t>
-  </si>
-  <si>
-    <t>Toss 거래 아이디</t>
-  </si>
-  <si>
-    <t>TOSS_TRANSACTION_ID</t>
-  </si>
-  <si>
-    <t>VARCHAR(255)</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_REFUND</t>
-  </si>
-  <si>
-    <t>HCP_PAYMENT_REFUND_UID</t>
-  </si>
-  <si>
     <t>HCP_PAYMENT 행 고유키</t>
   </si>
   <si>
@@ -599,7 +605,7 @@
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_INFO</t>
   </si>
   <si>
-    <t>대여 가능 상품 예약 결재 정보 고유키</t>
+    <t>대여 가능 상품 예약 결제 정보 고유키</t>
   </si>
 </sst>
 </file>
@@ -3506,7 +3512,7 @@
         <v>12</v>
       </c>
       <c r="H113" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="114">
@@ -3516,7 +3522,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116">
@@ -3553,7 +3559,7 @@
         <v>10</v>
       </c>
       <c r="C117" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
@@ -3628,7 +3634,7 @@
         <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C120" t="s">
         <v>150</v>
@@ -3654,25 +3660,25 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C121" t="s">
+        <v>169</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
+        <v>170</v>
+      </c>
+      <c r="F121" t="s">
+        <v>14</v>
+      </c>
+      <c r="G121" t="s">
+        <v>12</v>
+      </c>
+      <c r="H121" t="s">
         <v>168</v>
-      </c>
-      <c r="D121" t="s">
-        <v>12</v>
-      </c>
-      <c r="E121" t="s">
-        <v>169</v>
-      </c>
-      <c r="F121" t="s">
-        <v>14</v>
-      </c>
-      <c r="G121" t="s">
-        <v>12</v>
-      </c>
-      <c r="H121" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="122">
@@ -3680,25 +3686,25 @@
         <v>12</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C122" t="s">
+        <v>172</v>
+      </c>
+      <c r="D122" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" t="s">
+        <v>173</v>
+      </c>
+      <c r="F122" t="s">
+        <v>14</v>
+      </c>
+      <c r="G122" t="s">
+        <v>12</v>
+      </c>
+      <c r="H122" t="s">
         <v>171</v>
-      </c>
-      <c r="D122" t="s">
-        <v>12</v>
-      </c>
-      <c r="E122" t="s">
-        <v>172</v>
-      </c>
-      <c r="F122" t="s">
-        <v>14</v>
-      </c>
-      <c r="G122" t="s">
-        <v>12</v>
-      </c>
-      <c r="H122" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="123">
@@ -3706,25 +3712,25 @@
         <v>12</v>
       </c>
       <c r="B123" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C123" t="s">
+        <v>175</v>
+      </c>
+      <c r="D123" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" t="s">
+        <v>170</v>
+      </c>
+      <c r="F123" t="s">
+        <v>14</v>
+      </c>
+      <c r="G123" t="s">
+        <v>12</v>
+      </c>
+      <c r="H123" t="s">
         <v>174</v>
-      </c>
-      <c r="D123" t="s">
-        <v>12</v>
-      </c>
-      <c r="E123" t="s">
-        <v>169</v>
-      </c>
-      <c r="F123" t="s">
-        <v>14</v>
-      </c>
-      <c r="G123" t="s">
-        <v>12</v>
-      </c>
-      <c r="H123" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="124">
@@ -3734,7 +3740,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126">
@@ -3771,7 +3777,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -3846,7 +3852,7 @@
         <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C130" t="s">
         <v>150</v>
@@ -3872,25 +3878,25 @@
         <v>12</v>
       </c>
       <c r="B131" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C131" t="s">
+        <v>169</v>
+      </c>
+      <c r="D131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131" t="s">
+        <v>170</v>
+      </c>
+      <c r="F131" t="s">
+        <v>14</v>
+      </c>
+      <c r="G131" t="s">
+        <v>12</v>
+      </c>
+      <c r="H131" t="s">
         <v>168</v>
-      </c>
-      <c r="D131" t="s">
-        <v>12</v>
-      </c>
-      <c r="E131" t="s">
-        <v>169</v>
-      </c>
-      <c r="F131" t="s">
-        <v>14</v>
-      </c>
-      <c r="G131" t="s">
-        <v>12</v>
-      </c>
-      <c r="H131" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="132">
@@ -3898,16 +3904,16 @@
         <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C132" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
       </c>
       <c r="E132" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F132" t="s">
         <v>14</v>
@@ -3916,7 +3922,7 @@
         <v>12</v>
       </c>
       <c r="H132" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="133">
@@ -3924,25 +3930,25 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C133" t="s">
+        <v>175</v>
+      </c>
+      <c r="D133" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" t="s">
+        <v>170</v>
+      </c>
+      <c r="F133" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" t="s">
+        <v>12</v>
+      </c>
+      <c r="H133" t="s">
         <v>174</v>
-      </c>
-      <c r="D133" t="s">
-        <v>12</v>
-      </c>
-      <c r="E133" t="s">
-        <v>169</v>
-      </c>
-      <c r="F133" t="s">
-        <v>14</v>
-      </c>
-      <c r="G133" t="s">
-        <v>12</v>
-      </c>
-      <c r="H133" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="134">
@@ -3952,7 +3958,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="136">
@@ -3989,7 +3995,7 @@
         <v>10</v>
       </c>
       <c r="C137" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
@@ -4064,7 +4070,7 @@
         <v>23</v>
       </c>
       <c r="B140" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C140" t="s">
         <v>150</v>
@@ -4090,25 +4096,25 @@
         <v>12</v>
       </c>
       <c r="B141" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C141" t="s">
+        <v>183</v>
+      </c>
+      <c r="D141" t="s">
+        <v>12</v>
+      </c>
+      <c r="E141" t="s">
+        <v>184</v>
+      </c>
+      <c r="F141" t="s">
+        <v>14</v>
+      </c>
+      <c r="G141" t="s">
+        <v>12</v>
+      </c>
+      <c r="H141" t="s">
         <v>182</v>
-      </c>
-      <c r="D141" t="s">
-        <v>12</v>
-      </c>
-      <c r="E141" t="s">
-        <v>183</v>
-      </c>
-      <c r="F141" t="s">
-        <v>14</v>
-      </c>
-      <c r="G141" t="s">
-        <v>12</v>
-      </c>
-      <c r="H141" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="142">
@@ -4118,7 +4124,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="144">
@@ -4155,7 +4161,7 @@
         <v>10</v>
       </c>
       <c r="C145" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D145" t="s">
         <v>12</v>
@@ -4230,7 +4236,7 @@
         <v>23</v>
       </c>
       <c r="B148" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="C148" t="s">
         <v>150</v>
@@ -4248,7 +4254,7 @@
         <v>12</v>
       </c>
       <c r="H148" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149">
@@ -4256,10 +4262,10 @@
         <v>12</v>
       </c>
       <c r="B149" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C149" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D149" t="s">
         <v>12</v>
@@ -4274,7 +4280,7 @@
         <v>12</v>
       </c>
       <c r="H149" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="150">
@@ -4282,10 +4288,10 @@
         <v>12</v>
       </c>
       <c r="B150" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C150" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D150" t="s">
         <v>12</v>
@@ -4300,7 +4306,7 @@
         <v>12</v>
       </c>
       <c r="H150" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="151">
@@ -4308,10 +4314,10 @@
         <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C151" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D151" t="s">
         <v>12</v>
@@ -4326,7 +4332,7 @@
         <v>12</v>
       </c>
       <c r="H151" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="152">
@@ -4336,7 +4342,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154">
@@ -4373,7 +4379,7 @@
         <v>10</v>
       </c>
       <c r="C155" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D155" t="s">
         <v>12</v>
@@ -4448,7 +4454,7 @@
         <v>23</v>
       </c>
       <c r="B158" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C158" t="s">
         <v>11</v>
@@ -4474,7 +4480,7 @@
         <v>23</v>
       </c>
       <c r="B159" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C159" t="s">
         <v>150</v>
@@ -4492,7 +4498,7 @@
         <v>12</v>
       </c>
       <c r="H159" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="160">

</xml_diff>

<commit_message>
docs : ERD 자료 수정
</commit_message>
<xml_diff>
--- a/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
+++ b/module-service-rental-reservation/external_files/db/RentalReservation.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="223">
   <si>
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO</t>
   </si>
@@ -44,459 +44,468 @@
     <t>고유키</t>
   </si>
   <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO_UID</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>BIGINT UNSIGNED</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>행 고유키</t>
+  </si>
+  <si>
+    <t>삭제여부</t>
+  </si>
+  <si>
+    <t>DEL_FRAG</t>
+  </si>
+  <si>
+    <t>BIT(1)</t>
+  </si>
+  <si>
+    <t>행 삭제여부</t>
+  </si>
+  <si>
+    <t>행 생성일시</t>
+  </si>
+  <si>
+    <t>ROW_CREATE_DATETIME</t>
+  </si>
+  <si>
+    <t>DATETIME(3)</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 정보 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_INFO_UID</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_INFO 행 고유키</t>
+  </si>
+  <si>
+    <t>예약자 이름</t>
+  </si>
+  <si>
+    <t>CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>VARCHAR(90)</t>
+  </si>
+  <si>
+    <t>예약자 전화번호</t>
+  </si>
+  <si>
+    <t>CUSTOMER_PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>VARCHAR(45)</t>
+  </si>
+  <si>
+    <t>예약자 전화번호(국가번호 + 전화번호)</t>
+  </si>
+  <si>
+    <t>대여 시작 일시</t>
+  </si>
+  <si>
+    <t>RENTAL_START_DATETIME</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>대여가 시작되는 일시</t>
+  </si>
+  <si>
+    <t>대여 끝 일시</t>
+  </si>
+  <si>
+    <t>RENTAL_END_DATETIME</t>
+  </si>
+  <si>
+    <t>대여가 끝나는 일시 (회수 시간은 포함되지 않는 순수 서비스 이용 시간)</t>
+  </si>
+  <si>
+    <t>고객 예약 결제 기한</t>
+  </si>
+  <si>
+    <t>CUSTOMER_PAYMENT_DEADLINE_DATETIME</t>
+  </si>
+  <si>
+    <t>고객에게 이때까지 결제를 해야 한다고 통보한 기한</t>
+  </si>
+  <si>
+    <t>예약 결재 확인 기한</t>
+  </si>
+  <si>
+    <t>PAYMENT_CHECK_DEADLINE_DATETIME</t>
+  </si>
+  <si>
+    <t>예약 결재 확인 기한 (결재 기한 초과 처리.)</t>
+  </si>
+  <si>
+    <t>관리자 승인 기한</t>
+  </si>
+  <si>
+    <t>RESERVATION_APPROVAL_DEADLINE_DATETIME</t>
+  </si>
+  <si>
+    <t>관리자 승인 기한 (이 시점이 지났고, reservation_approval_datetime 가 충족되지 않았다면 취소로 간주)</t>
+  </si>
+  <si>
+    <t>예약 취소 가능 기한</t>
+  </si>
+  <si>
+    <t>RESERVATION_CANCEL_DEADLINE_DATETIME</t>
+  </si>
+  <si>
+    <t>상품명</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>고객에게 보일 상품명(아래 부터는 예약 당시의 정보로, 영수증의 기능을 위한 정보 복제 컬럼)</t>
+  </si>
+  <si>
+    <t>상품 소개</t>
+  </si>
+  <si>
+    <t>PRODUCT_INTRO</t>
+  </si>
+  <si>
+    <t>VARCHAR(6000)</t>
+  </si>
+  <si>
+    <t>고객에게 보일 상품 소개</t>
+  </si>
+  <si>
+    <t>상품 대표 이미지 테이블 고유번호</t>
+  </si>
+  <si>
+    <t>FRONT_IMAGE_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_IMAGE 행 고유키</t>
+  </si>
+  <si>
+    <t>주소-국가</t>
+  </si>
+  <si>
+    <t>ADDRESS_COUNTRY</t>
+  </si>
+  <si>
+    <t>VARCHAR(60)</t>
+  </si>
+  <si>
+    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 국가</t>
+  </si>
+  <si>
+    <t>주소-메인</t>
+  </si>
+  <si>
+    <t>ADDRESS_MAIN</t>
+  </si>
+  <si>
+    <t>VARCHAR(300)</t>
+  </si>
+  <si>
+    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 국가와 상세 주소를 제외</t>
+  </si>
+  <si>
+    <t>주소- 상세</t>
+  </si>
+  <si>
+    <t>ADDRESS_DETAIL</t>
+  </si>
+  <si>
+    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 상세</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO_UID</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 재고 카테고리 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_CATEGORY_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_CATEGORY 행 고유키</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 개별 설명</t>
+  </si>
+  <si>
+    <t>PRODUCT_DESC</t>
+  </si>
+  <si>
+    <t>VARCHAR(3000)</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 재고 이미지 테이블 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_IMAGE_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_IMAGE 행 고유키</t>
+  </si>
+  <si>
+    <t>제품 대여 가능 최초 일시</t>
+  </si>
+  <si>
+    <t>FIRST_RENTABLE_DATETIME</t>
+  </si>
+  <si>
+    <t>제품 대여(손님에게 제공)가 가능한 최초 일시</t>
+  </si>
+  <si>
+    <t>제품 대여 마지막 일시</t>
+  </si>
+  <si>
+    <t>LAST_RENTABLE_DATETIME</t>
+  </si>
+  <si>
+    <t>제품 대여 마지막 일시 (이때가 대여 마지막 날)</t>
+  </si>
+  <si>
+    <t>예약 가능 설정</t>
+  </si>
+  <si>
+    <t>NOW_RESERVABLE</t>
+  </si>
+  <si>
+    <t>재고, 상품 상태와 상관 없이 현 시점 예약 가능한지에 대한 관리자의 설정</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_INFO</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 카테고리 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_CATEGORY_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_CATEGORY 행 고유키</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 이미지 고유키</t>
+  </si>
+  <si>
+    <t>고객에게 보일 상품명</t>
+  </si>
+  <si>
+    <t>상품 예약 가능 최초 일시</t>
+  </si>
+  <si>
+    <t>FIRST_RESERVABLE_DATETIME</t>
+  </si>
+  <si>
+    <t>상품 예약이 가능한 최초 일시(콘서트 티켓 예매와 같은 서비스를 가정, 예약 러시 처리가 필요)</t>
+  </si>
+  <si>
+    <t>단위 예약 시간(분)</t>
+  </si>
+  <si>
+    <t>RESERVATION_UNIT_MINUTE</t>
+  </si>
+  <si>
+    <t>예약 추가 할 수 있는 최소 시간 단위 (분)</t>
+  </si>
+  <si>
+    <t>최소 예약 횟수</t>
+  </si>
+  <si>
+    <t>MINIMUM_RESERVATION_UNIT_COUNT</t>
+  </si>
+  <si>
+    <t>INT UNSIGNED</t>
+  </si>
+  <si>
+    <t>단위 예약 시간을 대여일 기준에서 최소 몇번 추가 해야 하는지</t>
+  </si>
+  <si>
+    <t>최대 예약 횟수</t>
+  </si>
+  <si>
+    <t>MAXIMUM_RESERVATION_UNIT_COUNT</t>
+  </si>
+  <si>
+    <t>단위 예약 시간을 대여일 기준에서 최대 몇번 추가 가능한지 (Null 이라면 제한 없음)</t>
+  </si>
+  <si>
+    <t>예약 단가</t>
+  </si>
+  <si>
+    <t>RESERVATION_UNIT_PRICE</t>
+  </si>
+  <si>
+    <t>DECIMAL(15, 2) UNSIGNED</t>
+  </si>
+  <si>
+    <t>단위 예약 시간에 대한 가격 (예약 시간 / 단위 예약 시간 * 예약 단가 = 예약 최종가)</t>
+  </si>
+  <si>
+    <t>예약 단가 통화 코드</t>
+  </si>
+  <si>
+    <t>RESERVATION_UNIT_PRICE_CURRENCY_CODE</t>
+  </si>
+  <si>
+    <t>CHAR(3)</t>
+  </si>
+  <si>
+    <t>단위 예약 시간에 대한 가격 통화 코드(IOS 4217, ex : KRW, USD, EUR...)</t>
+  </si>
+  <si>
+    <t>예약 상품 버전 시퀀스</t>
+  </si>
+  <si>
+    <t>VERSION_SEQ</t>
+  </si>
+  <si>
+    <t>예약 상품 정보 버전 시퀀스(고객이 정보를 확인한 시점의 버전과 예약 신청하는 시점의 버전이 다르면 진행 불가)</t>
+  </si>
+  <si>
+    <t>고객 결제 기한 설정값</t>
+  </si>
+  <si>
+    <t>CUSTOMER_PAYMENT_DEADLINE_MINUTE</t>
+  </si>
+  <si>
+    <t>고객에게 이때까지 결제를 해야 한다고 통보하는 기한 설정값(예약일로부터 +N 분)</t>
+  </si>
+  <si>
+    <t>결제 확인 기한 설정값</t>
+  </si>
+  <si>
+    <t>PAYMENT_CHECK_DEADLINE_MINUTE</t>
+  </si>
+  <si>
+    <t>관리자의 결제 확인 기한 설정값(예약일로 부터 +N 분, 고객 결제 기한 설정값보다 크거나 같음)</t>
+  </si>
+  <si>
+    <t>관리자 승인 기한 설정값</t>
+  </si>
+  <si>
+    <t>APPROVAL_DEADLINE_MINUTE</t>
+  </si>
+  <si>
+    <t>관리자의 예약 승인 기한 설정값(예약일로부터 +N분, 결제 확인 기한 설정값보다 크거나 같음)</t>
+  </si>
+  <si>
+    <t>취소 가능 기한 설정값</t>
+  </si>
+  <si>
+    <t>CANCEL_DEADLINE_MINUTE</t>
+  </si>
+  <si>
+    <t>고객이 예약 취소 가능한 기한 설정값(대여 시작일로부터 -N분이며, 그 결과가 관리자 승인 기한보다 커야함)</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY_UID</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 예약 정보 고유키</t>
+  </si>
+  <si>
     <t>HCP_PRODUCT_RESERVATION_INFO_UID</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>BIGINT UNSIGNED</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>행 고유키</t>
-  </si>
-  <si>
-    <t>삭제여부</t>
-  </si>
-  <si>
-    <t>DEL_FRAG</t>
-  </si>
-  <si>
-    <t>BIT(1)</t>
-  </si>
-  <si>
-    <t>행 삭제여부</t>
-  </si>
-  <si>
-    <t>행 생성일시</t>
-  </si>
-  <si>
-    <t>ROW_CREATE_DATETIME</t>
-  </si>
-  <si>
-    <t>DATETIME(3)</t>
-  </si>
-  <si>
-    <t>FK</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 정보 고유키</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_INFO_UID</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_INFO 행 고유키</t>
-  </si>
-  <si>
-    <t>예약자 이름</t>
-  </si>
-  <si>
-    <t>CUSTOMER_NAME</t>
-  </si>
-  <si>
-    <t>VARCHAR(90)</t>
-  </si>
-  <si>
-    <t>예약자 전화번호</t>
-  </si>
-  <si>
-    <t>CUSTOMER_PHONE_NUMBER</t>
-  </si>
-  <si>
-    <t>VARCHAR(45)</t>
-  </si>
-  <si>
-    <t>예약자 전화번호(국가번호 + 전화번호)</t>
-  </si>
-  <si>
-    <t>대여 시작 일시</t>
-  </si>
-  <si>
-    <t>RENTAL_START_DATETIME</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>대여가 시작되는 일시</t>
-  </si>
-  <si>
-    <t>대여 끝 일시</t>
-  </si>
-  <si>
-    <t>RENTAL_END_DATETIME</t>
-  </si>
-  <si>
-    <t>대여가 끝나는 일시 (회수 시간은 포함되지 않는 순수 서비스 이용 시간)</t>
-  </si>
-  <si>
-    <t>고객 예약 결제 기한</t>
-  </si>
-  <si>
-    <t>CUSTOMER_PAYMENT_DEADLINE_DATETIME</t>
-  </si>
-  <si>
-    <t>고객에게 이때까지 결제를 해야 한다고 통보한 기한</t>
-  </si>
-  <si>
-    <t>예약 결재 확인 기한</t>
-  </si>
-  <si>
-    <t>PAYMENT_CHECK_DEADLINE_DATETIME</t>
-  </si>
-  <si>
-    <t>예약 결재 확인 기한 (결재 기한 초과 처리.)</t>
-  </si>
-  <si>
-    <t>관리자 승인 기한</t>
-  </si>
-  <si>
-    <t>RESERVATION_APPROVAL_DEADLINE_DATETIME</t>
-  </si>
-  <si>
-    <t>관리자 승인 기한 (이 시점이 지났고, reservation_approval_datetime 가 충족되지 않았다면 취소로 간주)</t>
-  </si>
-  <si>
-    <t>예약 취소 가능 기한</t>
-  </si>
-  <si>
-    <t>RESERVATION_CANCEL_DEADLINE_DATETIME</t>
-  </si>
-  <si>
-    <t>상품명</t>
-  </si>
-  <si>
-    <t>PRODUCT_NAME</t>
-  </si>
-  <si>
-    <t>고객에게 보일 상품명(아래 부터는 예약 당시의 정보로, 영수증의 기능을 위한 정보 복제 컬럼)</t>
-  </si>
-  <si>
-    <t>상품 소개</t>
-  </si>
-  <si>
-    <t>PRODUCT_INTRO</t>
-  </si>
-  <si>
-    <t>VARCHAR(6000)</t>
-  </si>
-  <si>
-    <t>고객에게 보일 상품 소개</t>
-  </si>
-  <si>
-    <t>상품 대표 이미지 테이블 고유번호</t>
-  </si>
-  <si>
-    <t>FRONT_IMAGE_UID</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_IMAGE 행 고유키</t>
-  </si>
-  <si>
-    <t>주소-국가</t>
-  </si>
-  <si>
-    <t>ADDRESS_COUNTRY</t>
-  </si>
-  <si>
-    <t>VARCHAR(60)</t>
-  </si>
-  <si>
-    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 국가</t>
-  </si>
-  <si>
-    <t>주소-메인</t>
-  </si>
-  <si>
-    <t>ADDRESS_MAIN</t>
-  </si>
-  <si>
-    <t>VARCHAR(300)</t>
-  </si>
-  <si>
-    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 국가와 상세 주소를 제외</t>
-  </si>
-  <si>
-    <t>주소- 상세</t>
-  </si>
-  <si>
-    <t>ADDRESS_DETAIL</t>
-  </si>
-  <si>
-    <t>상품이 위치한 주소(대여 가능 위치의 기준으로 사용됨) - 상세</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO_UID</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 재고 카테고리 고유키</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_CATEGORY_UID</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_CATEGORY 행 고유키</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 개별 설명</t>
-  </si>
-  <si>
-    <t>PRODUCT_DESC</t>
-  </si>
-  <si>
-    <t>VARCHAR(3000)</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 재고 이미지 테이블 고유키</t>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO 행 고유키</t>
+  </si>
+  <si>
+    <t>예약 상태 코드</t>
+  </si>
+  <si>
+    <t>STATE_CODE</t>
+  </si>
+  <si>
+    <t>TINYINT UNSIGNED</t>
+  </si>
+  <si>
+    <t>예약 상태 코드(0 : 관리자 결제 확인, 1 : 관리자 예약 승인, 2 : 관리자 예약 거부, 3 : 사용자 예약 취소 신청, 4 : 관리자 예약 취소 승인, 5 : 예약 취소 거부, 6: 사용자 조기반납신고, 7: 관리자 조기반납 확인, 8: 결제 환불 처리)</t>
+  </si>
+  <si>
+    <t>상태 변경 상세</t>
+  </si>
+  <si>
+    <t>STATE_CHANGE_DESC</t>
+  </si>
+  <si>
+    <t>VARCHAR(600)</t>
+  </si>
+  <si>
+    <t>상태 변경 일시</t>
+  </si>
+  <si>
+    <t>STATE_CHANGE_DATETIME</t>
+  </si>
+  <si>
+    <t>상태 변경 기준 일시(행 생성일과 다르게 사건의 발생 일시 기준)</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_RESERVATION_INFO</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_RESERVATION_INFO_UID</t>
+  </si>
+  <si>
+    <t>대여 가능 상품 재고 정보 고유키</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO 행 고유키</t>
+  </si>
+  <si>
+    <t>다음 준비 예정일</t>
+  </si>
+  <si>
+    <t>NEXT_READY_DATETIME</t>
+  </si>
+  <si>
+    <t>다음 준비 예정일(예약 후 상품의 다음 고객의 대여까지 준비가 완료되는 일시, 이 값이 null 이라면 다음 예약이 불가)</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_CATEGORY</t>
+  </si>
+  <si>
+    <t>카테고리 이름</t>
+  </si>
+  <si>
+    <t>CATEGORY_NAME</t>
+  </si>
+  <si>
+    <t>부모 카테고리 고유키</t>
+  </si>
+  <si>
+    <t>PARENT_CATETORY_UID</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_IMAGE</t>
   </si>
   <si>
     <t>HCP_RENTABLE_PRODUCT_IMAGE_UID</t>
   </si>
   <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_IMAGE 행 고유키</t>
-  </si>
-  <si>
-    <t>제품 대여 가능 최초 일시</t>
-  </si>
-  <si>
-    <t>FIRST_RENTABLE_DATETIME</t>
-  </si>
-  <si>
-    <t>제품 대여(손님에게 제공)가 가능한 최초 일시</t>
-  </si>
-  <si>
-    <t>제품 대여 마지막 일시</t>
-  </si>
-  <si>
-    <t>LAST_RENTABLE_DATETIME</t>
-  </si>
-  <si>
-    <t>제품 대여 마지막 일시 (이때가 대여 마지막 날)</t>
-  </si>
-  <si>
-    <t>예약 가능 설정</t>
-  </si>
-  <si>
-    <t>NOW_RESERVABLE</t>
-  </si>
-  <si>
-    <t>재고, 상품 상태와 상관 없이 현 시점 예약 가능한지에 대한 관리자의 설정</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_INFO</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 카테고리 고유키</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_CATEGORY 행 고유키</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 이미지 고유키</t>
-  </si>
-  <si>
-    <t>고객에게 보일 상품명</t>
-  </si>
-  <si>
-    <t>상품 예약 가능 최초 일시</t>
-  </si>
-  <si>
-    <t>FIRST_RESERVABLE_DATETIME</t>
-  </si>
-  <si>
-    <t>상품 예약이 가능한 최초 일시(콘서트 티켓 예매와 같은 서비스를 가정, 예약 러시 처리가 필요)</t>
-  </si>
-  <si>
-    <t>단위 예약 시간(분)</t>
-  </si>
-  <si>
-    <t>RESERVATION_UNIT_MINUTE</t>
-  </si>
-  <si>
-    <t>예약 추가 할 수 있는 최소 시간 단위 (분)</t>
-  </si>
-  <si>
-    <t>최소 예약 횟수</t>
-  </si>
-  <si>
-    <t>MINIMUM_RESERVATION_UNIT_COUNT</t>
-  </si>
-  <si>
-    <t>INT UNSIGNED</t>
-  </si>
-  <si>
-    <t>단위 예약 시간을 대여일 기준에서 최소 몇번 추가 해야 하는지</t>
-  </si>
-  <si>
-    <t>최대 예약 횟수</t>
-  </si>
-  <si>
-    <t>MAXIMUM_RESERVATION_UNIT_COUNT</t>
-  </si>
-  <si>
-    <t>단위 예약 시간을 대여일 기준에서 최대 몇번 추가 가능한지 (Null 이라면 제한 없음)</t>
-  </si>
-  <si>
-    <t>예약 단가</t>
-  </si>
-  <si>
-    <t>RESERVATION_UNIT_PRICE</t>
-  </si>
-  <si>
-    <t>DECIMAL(15, 2) UNSIGNED</t>
-  </si>
-  <si>
-    <t>단위 예약 시간에 대한 가격 (예약 시간 / 단위 예약 시간 * 예약 단가 = 예약 최종가)</t>
-  </si>
-  <si>
-    <t>예약 단가 통화 코드</t>
-  </si>
-  <si>
-    <t>RESERVATION_UNIT_PRICE_CURRENCY_CODE</t>
-  </si>
-  <si>
-    <t>CHAR(3)</t>
-  </si>
-  <si>
-    <t>단위 예약 시간에 대한 가격 통화 코드(IOS 4217, ex : KRW, USD, EUR...)</t>
-  </si>
-  <si>
-    <t>예약 상품 버전 시퀀스</t>
-  </si>
-  <si>
-    <t>VERSION_SEQ</t>
-  </si>
-  <si>
-    <t>예약 상품 정보 버전 시퀀스(고객이 정보를 확인한 시점의 버전과 예약 신청하는 시점의 버전이 다르면 진행 불가)</t>
-  </si>
-  <si>
-    <t>고객 결제 기한 설정값</t>
-  </si>
-  <si>
-    <t>CUSTOMER_PAYMENT_DEADLINE_MINUTE</t>
-  </si>
-  <si>
-    <t>고객에게 이때까지 결제를 해야 한다고 통보하는 기한 설정값(예약일로부터 +N 분)</t>
-  </si>
-  <si>
-    <t>결제 확인 기한 설정값</t>
-  </si>
-  <si>
-    <t>PAYMENT_CHECK_DEADLINE_MINUTE</t>
-  </si>
-  <si>
-    <t>관리자의 결제 확인 기한 설정값(예약일로 부터 +N 분, 고객 결제 기한 설정값보다 크거나 같음)</t>
-  </si>
-  <si>
-    <t>관리자 승인 기한 설정값</t>
-  </si>
-  <si>
-    <t>APPROVAL_DEADLINE_MINUTE</t>
-  </si>
-  <si>
-    <t>관리자의 예약 승인 기한 설정값(예약일로부터 +N분, 결제 확인 기한 설정값보다 크거나 같음)</t>
-  </si>
-  <si>
-    <t>취소 가능 기한 설정값</t>
-  </si>
-  <si>
-    <t>CANCEL_DEADLINE_MINUTE</t>
-  </si>
-  <si>
-    <t>고객이 예약 취소 가능한 기한 설정값(대여 시작일로부터 -N분이며, 그 결과가 관리자 승인 기한보다 커야함)</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_STATE_CHANGE_HISTORY_UID</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 예약 정보 고유키</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_RESERVATION_INFO 행 고유키</t>
-  </si>
-  <si>
-    <t>예약 상태 코드</t>
-  </si>
-  <si>
-    <t>STATE_CODE</t>
-  </si>
-  <si>
-    <t>TINYINT UNSIGNED</t>
-  </si>
-  <si>
-    <t>예약 상태 코드(0 : 관리자 결제 확인, 1 : 관리자 예약 승인, 2 : 관리자 예약 거부, 3 : 사용자 예약 취소 신청, 4 : 관리자 예약 취소 승인, 5 : 예약 취소 거부, 6: 사용자 조기반납신고, 7: 관리자 조기반납 확인, 8: 결제 환불 처리)</t>
-  </si>
-  <si>
-    <t>상태 변경 상세</t>
-  </si>
-  <si>
-    <t>STATE_CHANGE_DESC</t>
-  </si>
-  <si>
-    <t>VARCHAR(600)</t>
-  </si>
-  <si>
-    <t>상태 변경 일시</t>
-  </si>
-  <si>
-    <t>STATE_CHANGE_DATETIME</t>
-  </si>
-  <si>
-    <t>상태 변경 기준 일시(행 생성일과 다르게 사건의 발생 일시 기준)</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_RESERVATION_INFO</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_RESERVATION_INFO_UID</t>
-  </si>
-  <si>
-    <t>대여 가능 상품 재고 정보 고유키</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_STOCK_INFO 행 고유키</t>
-  </si>
-  <si>
-    <t>다음 준비 예정일</t>
-  </si>
-  <si>
-    <t>NEXT_READY_DATETIME</t>
-  </si>
-  <si>
-    <t>다음 준비 예정일(예약 후 상품의 다음 고객의 대여까지 준비가 완료되는 일시, 이 값이 null 이라면 다음 예약이 불가)</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_CATEGORY</t>
-  </si>
-  <si>
-    <t>카테고리 이름</t>
-  </si>
-  <si>
-    <t>CATEGORY_NAME</t>
-  </si>
-  <si>
-    <t>부모 카테고리 고유키</t>
-  </si>
-  <si>
-    <t>PARENT_CATETORY_UID</t>
-  </si>
-  <si>
-    <t>HCP_RENTABLE_PRODUCT_IMAGE</t>
-  </si>
-  <si>
     <t>상품 이미지 Full URL</t>
   </si>
   <si>
@@ -521,7 +530,7 @@
     <t>HCP_PAYMENT</t>
   </si>
   <si>
-    <t>HCP_HCP_PAYMENT_UID</t>
+    <t>HCP_PAYMENT_UID</t>
   </si>
   <si>
     <t>결제 타입</t>
@@ -663,6 +672,9 @@
   </si>
   <si>
     <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_INFO</t>
+  </si>
+  <si>
+    <t>HCP_RENTABLE_PRODUCT_RESERVATION_PAYMENT_INFO_UID</t>
   </si>
   <si>
     <t>대여 가능 상품 예약 결제 정보 고유키</t>
@@ -1953,7 +1965,7 @@
         <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1968,7 +1980,7 @@
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41">
@@ -1976,7 +1988,7 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
         <v>61</v>
@@ -2020,7 +2032,7 @@
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43">
@@ -2132,10 +2144,10 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -2150,7 +2162,7 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48">
@@ -2158,10 +2170,10 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -2176,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49">
@@ -2184,16 +2196,16 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F49" t="s">
         <v>14</v>
@@ -2202,7 +2214,7 @@
         <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50">
@@ -2210,16 +2222,16 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F50" t="s">
         <v>26</v>
@@ -2228,7 +2240,7 @@
         <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51">
@@ -2236,16 +2248,16 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F51" t="s">
         <v>14</v>
@@ -2254,7 +2266,7 @@
         <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52">
@@ -2262,16 +2274,16 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F52" t="s">
         <v>14</v>
@@ -2280,7 +2292,7 @@
         <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53">
@@ -2314,10 +2326,10 @@
         <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -2332,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55">
@@ -2340,10 +2352,10 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
@@ -2358,7 +2370,7 @@
         <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56">
@@ -2366,10 +2378,10 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -2384,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57">
@@ -2392,10 +2404,10 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -2410,7 +2422,7 @@
         <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58">
@@ -2418,10 +2430,10 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -2436,7 +2448,7 @@
         <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59">
@@ -2446,7 +2458,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61">
@@ -2483,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -2558,10 +2570,10 @@
         <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="D65" t="s">
         <v>12</v>
@@ -2576,7 +2588,7 @@
         <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66">
@@ -2584,16 +2596,16 @@
         <v>12</v>
       </c>
       <c r="B66" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F66" t="s">
         <v>14</v>
@@ -2602,7 +2614,7 @@
         <v>12</v>
       </c>
       <c r="H66" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67">
@@ -2610,25 +2622,25 @@
         <v>12</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
       <c r="E67" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" t="s">
         <v>145</v>
-      </c>
-      <c r="F67" t="s">
-        <v>14</v>
-      </c>
-      <c r="G67" t="s">
-        <v>12</v>
-      </c>
-      <c r="H67" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="68">
@@ -2636,10 +2648,10 @@
         <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2654,7 +2666,7 @@
         <v>12</v>
       </c>
       <c r="H68" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69">
@@ -2664,7 +2676,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71">
@@ -2701,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -2776,7 +2788,7 @@
         <v>23</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
         <v>75</v>
@@ -2794,7 +2806,7 @@
         <v>12</v>
       </c>
       <c r="H75" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76">
@@ -2802,7 +2814,7 @@
         <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -2820,7 +2832,7 @@
         <v>12</v>
       </c>
       <c r="H76" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77">
@@ -2828,10 +2840,10 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C77" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -2846,7 +2858,7 @@
         <v>12</v>
       </c>
       <c r="H77" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78">
@@ -2856,7 +2868,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80">
@@ -2893,7 +2905,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
@@ -2968,10 +2980,10 @@
         <v>12</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C84" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -2986,7 +2998,7 @@
         <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85">
@@ -2994,10 +3006,10 @@
         <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -3012,7 +3024,7 @@
         <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86">
@@ -3022,7 +3034,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88">
@@ -3059,7 +3071,7 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
@@ -3160,16 +3172,16 @@
         <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F93" t="s">
         <v>14</v>
@@ -3178,7 +3190,7 @@
         <v>12</v>
       </c>
       <c r="H93" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94">
@@ -3188,7 +3200,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96">
@@ -3300,10 +3312,10 @@
         <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C100" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
@@ -3318,7 +3330,7 @@
         <v>12</v>
       </c>
       <c r="H100" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101">
@@ -3326,10 +3338,10 @@
         <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C101" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
@@ -3344,7 +3356,7 @@
         <v>12</v>
       </c>
       <c r="H101" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102">
@@ -3354,7 +3366,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="104">
@@ -3466,7 +3478,7 @@
         <v>23</v>
       </c>
       <c r="B108" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C108" t="s">
         <v>75</v>
@@ -3484,7 +3496,7 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109">
@@ -3492,16 +3504,16 @@
         <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C109" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
       </c>
       <c r="E109" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F109" t="s">
         <v>14</v>
@@ -3510,7 +3522,7 @@
         <v>12</v>
       </c>
       <c r="H109" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="110">
@@ -3520,7 +3532,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112">
@@ -3557,7 +3569,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -3632,16 +3644,16 @@
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C116" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
       </c>
       <c r="E116" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F116" t="s">
         <v>14</v>
@@ -3650,7 +3662,7 @@
         <v>12</v>
       </c>
       <c r="H116" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117">
@@ -3658,16 +3670,16 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C117" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F117" t="s">
         <v>14</v>
@@ -3676,7 +3688,7 @@
         <v>12</v>
       </c>
       <c r="H117" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118">
@@ -3684,16 +3696,16 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C118" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
       </c>
       <c r="E118" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F118" t="s">
         <v>14</v>
@@ -3702,7 +3714,7 @@
         <v>12</v>
       </c>
       <c r="H118" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119">
@@ -3710,10 +3722,10 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C119" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D119" t="s">
         <v>12</v>
@@ -3728,7 +3740,7 @@
         <v>12</v>
       </c>
       <c r="H119" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120">
@@ -3736,10 +3748,10 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C120" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D120" t="s">
         <v>12</v>
@@ -3754,7 +3766,7 @@
         <v>12</v>
       </c>
       <c r="H120" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="121">
@@ -3764,7 +3776,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123">
@@ -3801,7 +3813,7 @@
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D124" t="s">
         <v>12</v>
@@ -3876,10 +3888,10 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C127" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D127" t="s">
         <v>12</v>
@@ -3902,16 +3914,16 @@
         <v>12</v>
       </c>
       <c r="B128" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C128" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D128" t="s">
         <v>12</v>
       </c>
       <c r="E128" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F128" t="s">
         <v>14</v>
@@ -3920,7 +3932,7 @@
         <v>12</v>
       </c>
       <c r="H128" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129">
@@ -3928,16 +3940,16 @@
         <v>12</v>
       </c>
       <c r="B129" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C129" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D129" t="s">
         <v>12</v>
       </c>
       <c r="E129" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F129" t="s">
         <v>14</v>
@@ -3946,7 +3958,7 @@
         <v>12</v>
       </c>
       <c r="H129" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="130">
@@ -3954,16 +3966,16 @@
         <v>12</v>
       </c>
       <c r="B130" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C130" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>
       </c>
       <c r="E130" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F130" t="s">
         <v>14</v>
@@ -3972,7 +3984,7 @@
         <v>12</v>
       </c>
       <c r="H130" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131">
@@ -3982,7 +3994,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133">
@@ -4019,7 +4031,7 @@
         <v>10</v>
       </c>
       <c r="C134" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D134" t="s">
         <v>12</v>
@@ -4094,10 +4106,10 @@
         <v>23</v>
       </c>
       <c r="B137" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C137" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D137" t="s">
         <v>12</v>
@@ -4120,16 +4132,16 @@
         <v>12</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C138" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D138" t="s">
         <v>12</v>
       </c>
       <c r="E138" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F138" t="s">
         <v>14</v>
@@ -4138,7 +4150,7 @@
         <v>12</v>
       </c>
       <c r="H138" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139">
@@ -4146,16 +4158,16 @@
         <v>12</v>
       </c>
       <c r="B139" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C139" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D139" t="s">
         <v>12</v>
       </c>
       <c r="E139" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F139" t="s">
         <v>14</v>
@@ -4164,7 +4176,7 @@
         <v>12</v>
       </c>
       <c r="H139" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="140">
@@ -4172,16 +4184,16 @@
         <v>12</v>
       </c>
       <c r="B140" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C140" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D140" t="s">
         <v>12</v>
       </c>
       <c r="E140" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F140" t="s">
         <v>14</v>
@@ -4190,7 +4202,7 @@
         <v>12</v>
       </c>
       <c r="H140" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141">
@@ -4200,7 +4212,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143">
@@ -4237,7 +4249,7 @@
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D144" t="s">
         <v>12</v>
@@ -4312,10 +4324,10 @@
         <v>23</v>
       </c>
       <c r="B147" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C147" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D147" t="s">
         <v>12</v>
@@ -4338,16 +4350,16 @@
         <v>12</v>
       </c>
       <c r="B148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C148" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D148" t="s">
         <v>12</v>
       </c>
       <c r="E148" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F148" t="s">
         <v>14</v>
@@ -4356,7 +4368,7 @@
         <v>12</v>
       </c>
       <c r="H148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="149">
@@ -4366,7 +4378,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151">
@@ -4403,7 +4415,7 @@
         <v>10</v>
       </c>
       <c r="C152" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D152" t="s">
         <v>12</v>
@@ -4478,10 +4490,10 @@
         <v>23</v>
       </c>
       <c r="B155" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C155" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D155" t="s">
         <v>12</v>
@@ -4496,7 +4508,7 @@
         <v>12</v>
       </c>
       <c r="H155" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156">
@@ -4504,16 +4516,16 @@
         <v>12</v>
       </c>
       <c r="B156" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C156" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D156" t="s">
         <v>12</v>
       </c>
       <c r="E156" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F156" t="s">
         <v>14</v>
@@ -4522,7 +4534,7 @@
         <v>12</v>
       </c>
       <c r="H156" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157">
@@ -4530,16 +4542,16 @@
         <v>12</v>
       </c>
       <c r="B157" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C157" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D157" t="s">
         <v>12</v>
       </c>
       <c r="E157" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F157" t="s">
         <v>26</v>
@@ -4548,7 +4560,7 @@
         <v>12</v>
       </c>
       <c r="H157" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="158">
@@ -4556,10 +4568,10 @@
         <v>12</v>
       </c>
       <c r="B158" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C158" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D158" t="s">
         <v>12</v>
@@ -4574,7 +4586,7 @@
         <v>12</v>
       </c>
       <c r="H158" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="159">
@@ -4584,7 +4596,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="161">
@@ -4621,7 +4633,7 @@
         <v>10</v>
       </c>
       <c r="C162" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="D162" t="s">
         <v>12</v>
@@ -4696,7 +4708,7 @@
         <v>23</v>
       </c>
       <c r="B165" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C165" t="s">
         <v>11</v>
@@ -4714,7 +4726,7 @@
         <v>12</v>
       </c>
       <c r="H165" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="166">
@@ -4722,10 +4734,10 @@
         <v>23</v>
       </c>
       <c r="B166" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C166" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D166" t="s">
         <v>12</v>
@@ -4740,7 +4752,7 @@
         <v>12</v>
       </c>
       <c r="H166" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167">

</xml_diff>